<commit_message>
Add possibility to upload car fines instead of parking fines
</commit_message>
<xml_diff>
--- a/test/test_Excel_upload_bad.xlsx
+++ b/test/test_Excel_upload_bad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Alex\Programming\Projects\GoModules\edriver-space\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355A82FA-9D00-43E8-AD35-02BAB5171AE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEB8EBA-8D96-45EF-9988-101910E8A419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1305" windowWidth="23190" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1305" windowWidth="23145" windowHeight="13200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -37,34 +37,10 @@
     <t>CarID</t>
   </si>
   <si>
-    <t>A34</t>
-  </si>
-  <si>
-    <t>B27</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
-    <t>C34</t>
-  </si>
-  <si>
-    <t>F23</t>
-  </si>
-  <si>
     <t>Photo URL</t>
-  </si>
-  <si>
-    <t>https://1</t>
-  </si>
-  <si>
-    <t>https://2</t>
-  </si>
-  <si>
-    <t>https://3</t>
-  </si>
-  <si>
-    <t>https://4</t>
   </si>
 </sst>
 </file>
@@ -489,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,45 +487,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4">
-        <v>44553.75</v>
-      </c>
-      <c r="C2" s="3">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3">
-        <v>500</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4">
-        <v>44550.56527777778</v>
-      </c>
-      <c r="C3" s="3">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -849,10 +805,6 @@
       <c r="D46" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{C29588F4-E4EF-4413-8B98-D7A4807F7522}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{CBEAC631-B6A0-4F13-9B49-57CD9160FDA2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -861,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5F5D97-A534-427B-BEE0-A50193466DC6}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,51 +836,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4">
-        <v>44549.333333333336</v>
-      </c>
-      <c r="C2" s="3">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3">
-        <v>50324</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4">
-        <v>44555.56527777778</v>
-      </c>
-      <c r="C3" s="3">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3">
-        <v>23453</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{37D13092-B8AF-402D-9B3B-A75F6B75E1E5}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{D7CF14FD-7212-47AD-AEC7-11FB1DB56309}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>